<commit_message>
add full function html template
</commit_message>
<xml_diff>
--- a/test/reg.xlsx
+++ b/test/reg.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480CF50A-8682-4D10-A1F1-B2B9436FA87E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134EB21E-D99E-4095-BBDB-8A1673965D92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
   <si>
     <t>Block</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -179,6 +179,50 @@
   </si>
   <si>
     <t>Rand</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID register</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clock register</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Timer register</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID field</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clock division</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clock frequency</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clock enable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Counter value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Timer enable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Timer start</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -587,7 +631,7 @@
   <dimension ref="A1:Q59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -676,6 +720,9 @@
       <c r="G4" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="J4" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="K5" t="s">
@@ -696,6 +743,9 @@
       <c r="P5">
         <v>1</v>
       </c>
+      <c r="Q5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="6" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E6" s="5" t="s">
@@ -707,6 +757,9 @@
       <c r="G6" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="J6" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="L6" s="6"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
@@ -728,6 +781,9 @@
       <c r="P7">
         <v>1</v>
       </c>
+      <c r="Q7" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="K8" s="2" t="s">
@@ -748,6 +804,9 @@
       <c r="P8">
         <v>1</v>
       </c>
+      <c r="Q8" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="K9" s="2" t="s">
@@ -759,14 +818,17 @@
       <c r="M9" t="s">
         <v>12</v>
       </c>
-      <c r="N9">
-        <v>1</v>
+      <c r="N9" t="s">
+        <v>50</v>
       </c>
       <c r="O9">
         <v>1</v>
       </c>
       <c r="P9">
         <v>1</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -794,6 +856,9 @@
       <c r="I11" s="5">
         <v>4</v>
       </c>
+      <c r="J11" s="5" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="K12" s="2" t="s">
@@ -814,6 +879,9 @@
       <c r="P12">
         <v>1</v>
       </c>
+      <c r="Q12" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="K13" s="2" t="s">
@@ -834,6 +902,9 @@
       <c r="P13">
         <v>1</v>
       </c>
+      <c r="Q13" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="K14" s="2" t="s">
@@ -853,6 +924,9 @@
       </c>
       <c r="P14">
         <v>1</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">

</xml_diff>